<commit_message>
New sheet added into the Excel file
The "Sheet1" contains data which is used in simulation_new_data.py
</commit_message>
<xml_diff>
--- a/fitting_thomas_model_parameters.xlsx
+++ b/fitting_thomas_model_parameters.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\70073624\08_Projects\SAPD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlotte/Documents/Programming - Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC00F18-7070-6A43-A3FC-E6E7742972EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23040" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -107,8 +109,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,20 +388,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="5" max="5" width="41.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="3"/>
+    <col min="5" max="5" width="41.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -415,8 +415,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2">
@@ -428,22 +428,22 @@
       <c r="D2" s="1">
         <v>184.09884199999999</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
       <c r="B3">
         <v>67.5</v>
       </c>
       <c r="C3" s="1">
         <v>0.91343808299999996</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -455,22 +455,22 @@
       <c r="D4" s="1">
         <v>132.70118299999999</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
       <c r="B5">
         <v>67.5</v>
       </c>
       <c r="C5" s="1">
         <v>0.430702798</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6">
@@ -479,26 +479,25 @@
       <c r="C6" s="1">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="D6" s="6">
-        <v>159.04900000000001</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="1">
+        <v>159.04900000000001</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
       <c r="B7">
         <v>67.5</v>
       </c>
       <c r="C7" s="1">
         <v>0.77600000000000002</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -507,37 +506,35 @@
       <c r="C9" s="1">
         <v>0.22200600000000001</v>
       </c>
-      <c r="D9" s="6">
-        <v>159.04900000000001</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="1">
+        <v>159.04900000000001</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
       <c r="B10">
         <v>75.5</v>
       </c>
       <c r="C10" s="1">
         <v>0.54428100000000001</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
       <c r="B11">
         <v>78</v>
       </c>
       <c r="C11">
         <v>1.32799E-3</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B12">
@@ -549,37 +546,37 @@
       <c r="D12">
         <v>65.89</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
       <c r="B13">
         <v>75.5</v>
       </c>
       <c r="C13" s="1">
         <v>0.45500000000000002</v>
       </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
       <c r="B14">
         <v>78</v>
       </c>
       <c r="C14" s="1">
         <v>4.5599999999999998E-3</v>
       </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
       <c r="C15" s="1"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B16">
@@ -588,45 +585,45 @@
       <c r="C16" s="1">
         <v>0.63690000000000002</v>
       </c>
-      <c r="D16" s="6">
-        <v>159.04900000000001</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="1">
+        <v>159.04900000000001</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
       <c r="B17">
         <v>77</v>
       </c>
       <c r="C17" s="1">
         <v>0.19689999999999999</v>
       </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
       <c r="B18">
         <v>77.400000000000006</v>
       </c>
       <c r="C18" s="1">
         <v>0.40460000000000002</v>
       </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
       <c r="B19">
         <v>77.5</v>
       </c>
       <c r="C19" s="1">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B21">
@@ -635,35 +632,35 @@
       <c r="C21" s="1">
         <v>0.216</v>
       </c>
-      <c r="D21" s="6">
-        <v>159.04900000000001</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="1">
+        <v>159.04900000000001</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
       <c r="B22">
         <v>74.67</v>
       </c>
       <c r="C22" s="1">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
       <c r="B23">
         <v>75.89</v>
       </c>
       <c r="C23" s="1">
         <v>5.7624969899999996E-7</v>
       </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B25">
@@ -672,41 +669,35 @@
       <c r="C25" s="1">
         <v>0.49869999999999998</v>
       </c>
-      <c r="D25" s="6">
-        <v>159.04900000000001</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="1">
+        <v>159.04900000000001</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
       <c r="B26">
         <v>72.16</v>
       </c>
       <c r="C26" s="1">
         <v>0.51700000000000002</v>
       </c>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
       <c r="B27">
         <v>74.67</v>
       </c>
       <c r="C27" s="1">
         <v>8.8000000000000003E-4</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="E25:E27"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="E12:E14"/>
@@ -717,7 +708,164 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="E25:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CC5536-B9C7-FF43-81FE-B5F452A3CEE9}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>67.5</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0.77600000000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>72.06</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.49869999999999998</v>
+      </c>
+      <c r="C2" s="1">
+        <v>159.04900000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>72.16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.216</v>
+      </c>
+      <c r="C3" s="1">
+        <v>159.04900000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>72.16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.51700000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>74</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.22200600000000001</v>
+      </c>
+      <c r="C5" s="1">
+        <v>159.04900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>74.67</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7.1599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>74.67</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8.8000000000000003E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>75</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>159.04900000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>75.5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.54428100000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>75.5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.63690000000000002</v>
+      </c>
+      <c r="C10" s="1">
+        <v>159.04900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>75.89</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5.7624969899999996E-7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>77</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.19689999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.40460000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>77.5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>78</v>
+      </c>
+      <c r="B15">
+        <v>1.32799E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>